<commit_message>
update rent to 1785
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/572d0a92ad25842f/Documents/Budget API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{79BB131A-79AE-42EF-86EF-ED73B9B6A30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30AB7965-A98D-4554-B8FB-1B19FCE48DDC}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{79BB131A-79AE-42EF-86EF-ED73B9B6A30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{763E49E8-2A5C-4749-84ED-31D8139FE7A0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Kensey Nanny Griffin</t>
   </si>
   <si>
-    <t>chipolte</t>
-  </si>
-  <si>
     <t>Mint Mobile Kensey</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Kensey Classes</t>
   </si>
   <si>
-    <t>16800 saved per year</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -217,6 +211,12 @@
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>9600 saved per year</t>
+  </si>
+  <si>
+    <t>Eating out</t>
   </si>
 </sst>
 </file>
@@ -630,6 +630,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -835,8 +839,8 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -863,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -938,19 +942,19 @@
         <v>800</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E4" s="3">
         <v>160</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3">
         <v>20</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="6">
         <v>100</v>
@@ -958,21 +962,21 @@
     </row>
     <row r="5" spans="1:12" ht="14">
       <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <f>24.5*20*4</f>
+        <v>1960</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="3">
-        <f>24.5*25*4</f>
-        <v>2450</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="E5" s="3">
         <f>SUM(H2:H16)</f>
-        <v>880.96416666666676</v>
+        <v>890.96416666666676</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3">
         <v>20</v>
@@ -980,21 +984,21 @@
     </row>
     <row r="6" spans="1:12" ht="14">
       <c r="A6" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="24">
         <f>SUM(B2:B5)</f>
-        <v>7168.5599999999995</v>
+        <v>6678.5599999999995</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3">
         <f>SUM(K2:K4)</f>
         <v>250</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -1002,13 +1006,13 @@
     </row>
     <row r="7" spans="1:12" ht="14">
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3">
         <v>1000</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="3">
         <v>10</v>
@@ -1016,43 +1020,47 @@
     </row>
     <row r="8" spans="1:12" ht="14">
       <c r="D8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3">
         <v>250</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3">
         <f>K14</f>
         <v>333.84083333333331</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14">
       <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3">
+        <f>1735+F9</f>
+        <v>1785</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1735</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="H9" s="3">
         <v>50.29</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K9" s="17">
         <v>146.6</v>
@@ -1063,26 +1071,26 @@
     </row>
     <row r="10" spans="1:12" ht="14">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3">
         <f>SUM(H19:H20)</f>
         <v>600</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="3">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K10" s="17">
         <v>140</v>
@@ -1093,28 +1101,28 @@
     </row>
     <row r="11" spans="1:12" ht="14">
       <c r="A11" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="23">
         <f>B6</f>
-        <v>7168.5599999999995</v>
+        <v>6678.5599999999995</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="27">
         <f>SUM(E2:E10)</f>
-        <v>5655.9641666666666</v>
+        <v>5715.9641666666666</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="9">
         <f>130/12</f>
         <v>10.833333333333334</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K11" s="17">
         <v>30.28</v>
@@ -1125,21 +1133,21 @@
     </row>
     <row r="12" spans="1:12" ht="14">
       <c r="A12" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="25">
         <f>E11</f>
-        <v>5655.9641666666666</v>
+        <v>5715.9641666666666</v>
       </c>
       <c r="D12" s="10"/>
       <c r="G12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="3">
         <v>8</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" ref="K12:K13" si="0">L12/12</f>
@@ -1151,23 +1159,23 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="28">
         <f>B11-B12</f>
-        <v>1512.5958333333328</v>
+        <v>962.59583333333285</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="H13" s="3">
         <v>88</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="0"/>
@@ -1180,20 +1188,20 @@
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="11">
         <f>ROUND(B13,-2)-200</f>
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="13"/>
       <c r="G14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="3">
         <v>12</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K14" s="19">
         <f>SUM(K9:K13)</f>
@@ -1203,20 +1211,20 @@
     <row r="15" spans="1:12" ht="14">
       <c r="A15" s="11">
         <f>12*A14</f>
-        <v>15600</v>
+        <v>9600</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="E15" s="3">
         <f>H19</f>
         <v>300</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H15" s="3">
         <v>200</v>
@@ -1224,13 +1232,13 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="E16" s="3">
         <f>H11</f>
@@ -1242,13 +1250,13 @@
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
       <c r="A17" s="11">
         <f>A15</f>
-        <v>15600</v>
+        <v>9600</v>
       </c>
       <c r="B17" s="11">
         <v>1</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" s="1">
         <f>SUM(E15:E16)</f>
@@ -1258,31 +1266,31 @@
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
       <c r="A18" s="16">
         <f t="shared" ref="A18:A36" si="1">FV(0.08,1,,A17)*-1</f>
-        <v>16848</v>
+        <v>10368</v>
       </c>
       <c r="B18" s="11">
         <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="16">
         <f t="shared" si="1"/>
-        <v>18195.84</v>
+        <v>11197.44</v>
       </c>
       <c r="B19" s="11">
         <v>3</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="3">
         <f>600/2</f>
@@ -1292,17 +1300,17 @@
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="16">
         <f t="shared" si="1"/>
-        <v>19651.5072</v>
+        <v>12093.235200000001</v>
       </c>
       <c r="B20" s="11">
         <v>4</v>
       </c>
       <c r="D20" s="11">
         <f>SUM(A17:A21)</f>
-        <v>91518.974975999998</v>
+        <v>56319.369216000006</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H20" s="6">
         <v>300</v>
@@ -1311,7 +1319,7 @@
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="16">
         <f t="shared" si="1"/>
-        <v>21223.627776000001</v>
+        <v>13060.694016000001</v>
       </c>
       <c r="B21" s="11">
         <v>5</v>
@@ -1320,7 +1328,7 @@
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="16">
         <f t="shared" si="1"/>
-        <v>22921.517998080002</v>
+        <v>14105.549537280001</v>
       </c>
       <c r="B22" s="11">
         <v>6</v>
@@ -1329,32 +1337,32 @@
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
       <c r="A23" s="16">
         <f t="shared" si="1"/>
-        <v>24755.239437926404</v>
+        <v>15233.993500262402</v>
       </c>
       <c r="B23" s="11">
         <v>7</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.5">
       <c r="A24" s="16">
         <f t="shared" si="1"/>
-        <v>26735.658592960517</v>
+        <v>16452.712980283395</v>
       </c>
       <c r="B24" s="11">
         <v>8</v>
       </c>
       <c r="D24" s="11">
         <f>SUM(A17:A26)</f>
-        <v>225990.37446819345</v>
+        <v>139070.99967273444</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="12.5">
       <c r="A25" s="16">
         <f t="shared" si="1"/>
-        <v>28874.511280397361</v>
+        <v>17768.930018706069</v>
       </c>
       <c r="B25" s="11">
         <v>9</v>
@@ -1363,7 +1371,7 @@
     <row r="26" spans="1:8" ht="12.5">
       <c r="A26" s="16">
         <f t="shared" si="1"/>
-        <v>31184.472182829151</v>
+        <v>19190.444420202555</v>
       </c>
       <c r="B26" s="11">
         <f t="shared" ref="B26:B36" si="2">B25+1</f>
@@ -1373,7 +1381,7 @@
     <row r="27" spans="1:8" ht="12.5">
       <c r="A27" s="16">
         <f t="shared" si="1"/>
-        <v>33679.229957455485</v>
+        <v>20725.679973818762</v>
       </c>
       <c r="B27" s="11">
         <f t="shared" si="2"/>
@@ -1383,20 +1391,20 @@
     <row r="28" spans="1:8" ht="12.5">
       <c r="A28" s="16">
         <f t="shared" si="1"/>
-        <v>36373.568354051924</v>
+        <v>22383.734371724266</v>
       </c>
       <c r="B28" s="11">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.5">
       <c r="A29" s="16">
         <f t="shared" si="1"/>
-        <v>39283.453822376083</v>
+        <v>24174.433121462207</v>
       </c>
       <c r="B29" s="11">
         <f t="shared" si="2"/>
@@ -1404,13 +1412,13 @@
       </c>
       <c r="D29" s="11">
         <f>SUM(A17:A31)</f>
-        <v>423572.97726866254</v>
+        <v>260660.29370379238</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.5">
       <c r="A30" s="16">
         <f t="shared" si="1"/>
-        <v>42426.130128166173</v>
+        <v>26108.387771179187</v>
       </c>
       <c r="B30" s="11">
         <f t="shared" si="2"/>
@@ -1420,7 +1428,7 @@
     <row r="31" spans="1:8" ht="12.5">
       <c r="A31" s="16">
         <f t="shared" si="1"/>
-        <v>45820.220538419468</v>
+        <v>28197.058792873522</v>
       </c>
       <c r="B31" s="11">
         <f t="shared" si="2"/>
@@ -1430,7 +1438,7 @@
     <row r="32" spans="1:8" ht="12.5">
       <c r="A32" s="16">
         <f t="shared" si="1"/>
-        <v>49485.838181493025</v>
+        <v>30452.823496303405</v>
       </c>
       <c r="B32" s="11">
         <f t="shared" si="2"/>
@@ -1440,20 +1448,20 @@
     <row r="33" spans="1:4" ht="12.5">
       <c r="A33" s="16">
         <f t="shared" si="1"/>
-        <v>53444.705236012473</v>
+        <v>32889.049376007679</v>
       </c>
       <c r="B33" s="11">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.5">
       <c r="A34" s="16">
         <f t="shared" si="1"/>
-        <v>57720.281654893472</v>
+        <v>35520.173326088297</v>
       </c>
       <c r="B34" s="11">
         <f t="shared" si="2"/>
@@ -1461,13 +1469,13 @@
       </c>
       <c r="D34" s="11">
         <f>SUM(A17:A36)</f>
-        <v>713886.64305061428</v>
+        <v>439314.85726191651</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.5">
       <c r="A35" s="16">
         <f t="shared" si="1"/>
-        <v>62337.904187284956</v>
+        <v>38361.787192175361</v>
       </c>
       <c r="B35" s="11">
         <f t="shared" si="2"/>
@@ -1477,7 +1485,7 @@
     <row r="36" spans="1:4" ht="12.5">
       <c r="A36" s="16">
         <f t="shared" si="1"/>
-        <v>67324.936522267759</v>
+        <v>41430.730167549395</v>
       </c>
       <c r="B36" s="11">
         <f t="shared" si="2"/>
@@ -1493,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33500A77-C53B-4FDA-9242-DDA283C4C84C}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1523,7 +1531,7 @@
         <v>ENVELOPE DIS SHIT</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G1" s="33" t="str">
         <f>Sheet1!A10</f>
@@ -1534,7 +1542,7 @@
         <v>Amount</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="31" t="str">
         <f>Sheet1!H1</f>
@@ -1588,7 +1596,7 @@
       </c>
       <c r="H2" s="36">
         <f>Sheet1!B11</f>
-        <v>7168.5599999999995</v>
+        <v>6678.5599999999995</v>
       </c>
       <c r="J2" s="34" t="str">
         <f>Sheet1!G2</f>
@@ -1646,7 +1654,7 @@
       </c>
       <c r="H3" s="29">
         <f>Sheet1!B12</f>
-        <v>5655.9641666666666</v>
+        <v>5715.9641666666666</v>
       </c>
       <c r="J3" s="34" t="str">
         <f>Sheet1!G3</f>
@@ -1684,7 +1692,7 @@
     <row r="4" spans="1:20" ht="13" thickBot="1">
       <c r="A4" s="34" t="str">
         <f>Sheet1!D4</f>
-        <v>chipolte</v>
+        <v>Eating out</v>
       </c>
       <c r="B4" s="29">
         <f>Sheet1!E4</f>
@@ -1704,7 +1712,7 @@
       </c>
       <c r="H4" s="30">
         <f>Sheet1!B13</f>
-        <v>1512.5958333333328</v>
+        <v>962.59583333333285</v>
       </c>
       <c r="J4" s="34" t="str">
         <f>Sheet1!G4</f>
@@ -1738,7 +1746,7 @@
       </c>
       <c r="B5" s="29">
         <f>Sheet1!E5</f>
-        <v>880.96416666666676</v>
+        <v>890.96416666666676</v>
       </c>
       <c r="D5" s="33" t="str">
         <f>Sheet1!D17</f>
@@ -1846,7 +1854,7 @@
       </c>
       <c r="B9" s="29">
         <f>Sheet1!E9</f>
-        <v>1735</v>
+        <v>1785</v>
       </c>
       <c r="J9" s="34" t="str">
         <f>Sheet1!G9</f>
@@ -1872,7 +1880,7 @@
       </c>
       <c r="K10" s="29">
         <f>Sheet1!H10</f>
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="13" thickBot="1">
@@ -1882,7 +1890,7 @@
       </c>
       <c r="B11" s="31">
         <f>Sheet1!E11</f>
-        <v>5655.9641666666666</v>
+        <v>5715.9641666666666</v>
       </c>
       <c r="J11" s="34" t="str">
         <f>Sheet1!G11</f>
@@ -1945,11 +1953,11 @@
     </row>
     <row r="17" spans="10:11" ht="13" thickBot="1">
       <c r="J17" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K17" s="31">
         <f>SUM(K2:K16)</f>
-        <v>880.96416666666676</v>
+        <v>890.96416666666676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>